<commit_message>
Added New SA Module
</commit_message>
<xml_diff>
--- a/Config/SSO.xlsx
+++ b/Config/SSO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LouisVincentGalvez\MeralcoOnlinePortal\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4112BA0-4C23-459C-B87D-C8A1E70D25D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E1CA6A-06B5-4015-9922-D437E4EA31BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E544E56B-5137-4BEF-824C-37E29E8723E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E544E56B-5137-4BEF-824C-37E29E8723E4}"/>
   </bookViews>
   <sheets>
     <sheet name="AT - Test Suite" sheetId="5" r:id="rId1"/>
@@ -1016,6 +1016,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1023,18 +1035,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2304,8 +2304,8 @@
   </sheetPr>
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3651,8 +3651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A009D915-6C12-4050-90F7-83F7DCE02B67}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3912,14 +3912,14 @@
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="42"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
@@ -3954,14 +3954,14 @@
       <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="42"/>
     </row>
     <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
@@ -3996,14 +3996,14 @@
       <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
     </row>
     <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
@@ -4022,14 +4022,14 @@
       <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="42"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="46"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
@@ -4048,14 +4048,14 @@
       <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="42"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
@@ -4074,14 +4074,14 @@
       <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="42"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="46"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
@@ -4100,14 +4100,14 @@
       <c r="F30" s="16"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="46"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
@@ -4126,14 +4126,14 @@
       <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="42"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="46"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
@@ -4152,14 +4152,14 @@
       <c r="F34" s="16"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="42"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="46"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
@@ -4179,12 +4179,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A25:F25"/>
@@ -4192,6 +4186,12 @@
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4790,18 +4790,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4824,18 +4824,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4000A3CA-88F2-4739-B763-76748DB18036}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2585DB6-C699-4C2E-B17B-B2952AEF821E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4000A3CA-88F2-4739-B763-76748DB18036}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>